<commit_message>
changed alignement of column E (#1183)
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskz_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskz_vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerke\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67258A49-E840-4C47-A35A-97BB5C6866ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53EC290-DDB9-40AA-9167-8CA7AF78517D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="11610" windowHeight="10245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sskz" sheetId="6" r:id="rId1"/>
@@ -134,33 +134,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -184,9 +175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -224,9 +215,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,26 +250,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,26 +285,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -504,11 +461,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT52"/>
+  <dimension ref="B1:AT52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -527,24 +482,23 @@
     <col min="16" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="2:46" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="2"/>
@@ -587,482 +541,202 @@
       <c r="AS1" s="2"/>
       <c r="AT1" s="2"/>
     </row>
-    <row r="2" spans="1:46" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:46" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="5"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="5"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="5"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="5"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="5"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="5"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="5"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="5"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="H3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="4"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -1072,18 +746,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Nicht begonnen</_Status>
-    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1275,20 +937,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Nicht begonnen</_Status>
+    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1334,24 +995,20 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1177B4BE-B106-4A5F-9B8B-849CAD24B948}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD45C59E-C13E-4B92-9551-AE1790848EFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1370,10 +1027,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1177B4BE-B106-4A5F-9B8B-849CAD24B948}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1387,9 +1061,9 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sskz: Add notice column (#1264)
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskz_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskz_vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\SBIDER-Current\eclipse\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53EC290-DDB9-40AA-9167-8CA7AF78517D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8113962D-389C-4F21-B2C5-92F1408E19ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="11610" windowHeight="10245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sskz" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>A</t>
   </si>
@@ -61,6 +61,12 @@
   <si>
     <t>F</t>
   </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Bemerkung</t>
+  </si>
 </sst>
 </file>
 
@@ -94,7 +100,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -130,32 +136,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -175,9 +257,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,9 +297,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,9 +332,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,9 +384,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -461,18 +577,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AT52"/>
+  <dimension ref="A1:AT52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="D1" zoomScale="160" zoomScaleNormal="100" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="2" customWidth="1"/>
     <col min="2" max="3" width="24" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="78.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -482,26 +601,29 @@
     <col min="16" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:46" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:46" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -541,202 +663,485 @@
       <c r="AS1" s="2"/>
       <c r="AT1" s="2"/>
     </row>
-    <row r="2" spans="2:46" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:46" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="H3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F48" s="4"/>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="4"/>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F52" s="4"/>
+      <c r="H2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="15"/>
+      <c r="J3" s="4"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="5"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -746,6 +1151,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Nicht begonnen</_Status>
+    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -937,19 +1354,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Nicht begonnen</_Status>
-    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -995,20 +1413,24 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1177B4BE-B106-4A5F-9B8B-849CAD24B948}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD45C59E-C13E-4B92-9551-AE1790848EFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1027,27 +1449,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1177B4BE-B106-4A5F-9B8B-849CAD24B948}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1061,9 +1466,9 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>